<commit_message>
Added prefix for regions
</commit_message>
<xml_diff>
--- a/examples/WebIndexSimple/dataSimple0.4.xlsx
+++ b/examples/WebIndexSimple/dataSimple0.4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="7908" tabRatio="554" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="7908" tabRatio="554" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -3942,7 +3942,7 @@
   <sheetPr codeName="Hoja23"/>
   <dimension ref="A2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4658,7 +4658,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>266</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>263</v>
       </c>
@@ -5363,7 +5363,7 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added web foundation ontology
</commit_message>
<xml_diff>
--- a/examples/WebIndexSimple/dataSimple0.4.xlsx
+++ b/examples/WebIndexSimple/dataSimple0.4.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="7908" tabRatio="554" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="7908" tabRatio="554" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="A-RAW" sheetId="2" r:id="rId2"/>
     <sheet name="B-RAW" sheetId="6" r:id="rId3"/>
     <sheet name="C-RAW" sheetId="7" r:id="rId4"/>
-    <sheet name="Q1" sheetId="32" r:id="rId5"/>
-    <sheet name="Q2" sheetId="33" r:id="rId6"/>
-    <sheet name="D-Raw" sheetId="8" r:id="rId7"/>
+    <sheet name="D-Raw" sheetId="8" r:id="rId5"/>
+    <sheet name="Q1" sheetId="32" r:id="rId6"/>
+    <sheet name="Q2" sheetId="33" r:id="rId7"/>
     <sheet name="A-Imputed" sheetId="28" r:id="rId8"/>
     <sheet name="B-Imputed" sheetId="29" r:id="rId9"/>
     <sheet name="C-Imputed" sheetId="30" r:id="rId10"/>
@@ -31,7 +31,7 @@
     <sheet name="B-Normalised" sheetId="15" r:id="rId17"/>
     <sheet name="C-Normalised" sheetId="14" r:id="rId18"/>
     <sheet name="D-Normalised" sheetId="16" r:id="rId19"/>
-    <sheet name="Indicators-SelectYear" sheetId="21" r:id="rId20"/>
+    <sheet name="Indicators-Cluster" sheetId="21" r:id="rId20"/>
     <sheet name="Indicators-Adjusted" sheetId="24" r:id="rId21"/>
     <sheet name="Indicators-Weighted" sheetId="25" r:id="rId22"/>
     <sheet name="Clusters-Grouped" sheetId="22" r:id="rId23"/>
@@ -2859,7 +2859,7 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -4120,27 +4120,27 @@
         <v>204</v>
       </c>
       <c r="B2" s="5">
-        <f>'Indicators-SelectYear'!B3+8</f>
+        <f>'Indicators-Cluster'!B3+8</f>
         <v>8</v>
       </c>
       <c r="C2" s="5">
-        <f>'Indicators-SelectYear'!C3+8</f>
+        <f>'Indicators-Cluster'!C3+8</f>
         <v>7</v>
       </c>
       <c r="D2" s="5">
-        <f>'Indicators-SelectYear'!D3+8</f>
+        <f>'Indicators-Cluster'!D3+8</f>
         <v>9.1208970766356092</v>
       </c>
       <c r="E2" s="5">
-        <f>'Indicators-SelectYear'!E3+8</f>
+        <f>'Indicators-Cluster'!E3+8</f>
         <v>7.079684306331119</v>
       </c>
       <c r="F2" s="5">
-        <f>'Indicators-SelectYear'!F3+8</f>
+        <f>'Indicators-Cluster'!F3+8</f>
         <v>8.5773502691896262</v>
       </c>
       <c r="G2" s="5">
-        <f>'Indicators-SelectYear'!G3+8</f>
+        <f>'Indicators-Cluster'!G3+8</f>
         <v>7</v>
       </c>
     </row>
@@ -4149,27 +4149,27 @@
         <v>78</v>
       </c>
       <c r="B3" s="5">
-        <f>'Indicators-SelectYear'!B4+8</f>
+        <f>'Indicators-Cluster'!B4+8</f>
         <v>7</v>
       </c>
       <c r="C3" s="5">
-        <f>'Indicators-SelectYear'!C4+8</f>
+        <f>'Indicators-Cluster'!C4+8</f>
         <v>8</v>
       </c>
       <c r="D3" s="5">
-        <f>'Indicators-SelectYear'!D4+8</f>
+        <f>'Indicators-Cluster'!D4+8</f>
         <v>7.1993592309745642</v>
       </c>
       <c r="E3" s="5">
-        <f>'Indicators-SelectYear'!E4+8</f>
+        <f>'Indicators-Cluster'!E4+8</f>
         <v>7.8562006728642375</v>
       </c>
       <c r="F3" s="5">
-        <f>'Indicators-SelectYear'!F4+8</f>
+        <f>'Indicators-Cluster'!F4+8</f>
         <v>6.8452994616207476</v>
       </c>
       <c r="G3" s="5">
-        <f>'Indicators-SelectYear'!G4+8</f>
+        <f>'Indicators-Cluster'!G4+8</f>
         <v>8</v>
       </c>
     </row>
@@ -4178,27 +4178,27 @@
         <v>48</v>
       </c>
       <c r="B4" s="5">
-        <f>'Indicators-SelectYear'!B5+8</f>
+        <f>'Indicators-Cluster'!B5+8</f>
         <v>9</v>
       </c>
       <c r="C4" s="5">
-        <f>'Indicators-SelectYear'!C5+8</f>
+        <f>'Indicators-Cluster'!C5+8</f>
         <v>9</v>
       </c>
       <c r="D4" s="5">
-        <f>'Indicators-SelectYear'!D5+8</f>
+        <f>'Indicators-Cluster'!D5+8</f>
         <v>7.6797436923898257</v>
       </c>
       <c r="E4" s="5">
-        <f>'Indicators-SelectYear'!E5+8</f>
+        <f>'Indicators-Cluster'!E5+8</f>
         <v>9.0641150208046444</v>
       </c>
       <c r="F4" s="5">
-        <f>'Indicators-SelectYear'!F5+8</f>
+        <f>'Indicators-Cluster'!F5+8</f>
         <v>8.5773502691896262</v>
       </c>
       <c r="G4" s="5">
-        <f>'Indicators-SelectYear'!G5+8</f>
+        <f>'Indicators-Cluster'!G5+8</f>
         <v>9</v>
       </c>
     </row>
@@ -4398,7 +4398,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4512,7 +4512,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4596,7 +4596,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4653,7 +4653,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -5144,6 +5144,95 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="6">
+        <v>2009</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2010</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="13">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5250,7 +5339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:C10"/>
@@ -5350,95 +5439,6 @@
       <formula1>datatype</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="6">
-        <v>2009</v>
-      </c>
-      <c r="C1" s="6">
-        <v>2010</v>
-      </c>
-      <c r="D1" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="5">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="13">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
-        <v>6</v>
-      </c>
-      <c r="D4" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Computex ontology as RDF/XML syntax
</commit_message>
<xml_diff>
--- a/examples/WebIndexSimple/dataSimple0.4.xlsx
+++ b/examples/WebIndexSimple/dataSimple0.4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16536" windowHeight="7908" tabRatio="554" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="5664" tabRatio="554" firstSheet="22" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -31,27 +31,31 @@
     <sheet name="B-Normalised" sheetId="15" r:id="rId17"/>
     <sheet name="C-Normalised" sheetId="14" r:id="rId18"/>
     <sheet name="D-Normalised" sheetId="16" r:id="rId19"/>
-    <sheet name="Indicators-Cluster" sheetId="21" r:id="rId20"/>
-    <sheet name="Indicators-Adjusted" sheetId="24" r:id="rId21"/>
-    <sheet name="Indicators-Weighted" sheetId="25" r:id="rId22"/>
-    <sheet name="Clusters-Grouped" sheetId="22" r:id="rId23"/>
-    <sheet name="Subindex-Grouped" sheetId="26" r:id="rId24"/>
-    <sheet name="Composite" sheetId="27" r:id="rId25"/>
-    <sheet name="Rankings" sheetId="20" r:id="rId26"/>
-    <sheet name="Survey-Raw" sheetId="34" r:id="rId27"/>
-    <sheet name="Survey-Normalised" sheetId="35" r:id="rId28"/>
+    <sheet name="Indicators-Cluster-2010" sheetId="36" r:id="rId20"/>
+    <sheet name="Indicators-Weighted-2010" sheetId="37" r:id="rId21"/>
+    <sheet name="Clusters-Grouped-2010" sheetId="38" r:id="rId22"/>
+    <sheet name="Subindex-Grouped-2010" sheetId="39" r:id="rId23"/>
+    <sheet name="Composite-2010" sheetId="40" r:id="rId24"/>
+    <sheet name="Indicators-Cluster-2012" sheetId="21" r:id="rId25"/>
+    <sheet name="Indicators-Weighted-2012" sheetId="25" r:id="rId26"/>
+    <sheet name="Clusters-Grouped-2012" sheetId="22" r:id="rId27"/>
+    <sheet name="Subindex-Grouped-2012" sheetId="26" r:id="rId28"/>
+    <sheet name="Composite-2012" sheetId="27" r:id="rId29"/>
+    <sheet name="Rankings-2012" sheetId="20" r:id="rId30"/>
+    <sheet name="Survey-Raw" sheetId="34" r:id="rId31"/>
+    <sheet name="Survey-Normalised" sheetId="35" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="283">
   <si>
     <t>Raw</t>
   </si>
@@ -909,7 +913,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -992,6 +996,12 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1063,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1104,6 +1114,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2859,7 +2870,7 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -3684,7 +3695,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3770,7 +3781,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3939,128 +3950,97 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja23"/>
-  <dimension ref="A2:G5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>253</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C1" t="s">
         <v>254</v>
       </c>
-      <c r="D2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D1" t="s">
         <v>255</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E1" t="s">
         <v>256</v>
       </c>
-      <c r="G2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="5">
+        <f>'A-Normalised'!B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <f>'B-Normalised'!B$2</f>
+        <v>-1</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'C-Normalised'!B$2</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'D-Normalised'!B$2</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5">
-        <f>'A-Normalised'!D$2</f>
+        <f>'A-Normalised'!B3</f>
+        <v>-1</v>
+      </c>
+      <c r="C3" s="5">
+        <f>'B-Normalised'!B3</f>
         <v>0</v>
       </c>
-      <c r="C3" s="5">
-        <f>'B-Normalised'!D$2</f>
-        <v>-1</v>
-      </c>
       <c r="D3" s="5">
-        <f>'Survey-Normalised'!C$3</f>
-        <v>1.1208970766356094</v>
+        <f>'C-Normalised'!B3</f>
+        <v>-0.57735026918962551</v>
       </c>
       <c r="E3" s="5">
-        <f>'C-Normalised'!D$2</f>
-        <v>-0.92031569366888055</v>
-      </c>
-      <c r="F3" s="5">
-        <f>'D-Normalised'!D$2</f>
+        <f>'D-Normalised'!B3</f>
+        <v>-1.1547005383792521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'A-Normalised'!B4</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'B-Normalised'!B4</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'C-Normalised'!B4</f>
+        <v>1.1547005383792501</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'D-Normalised'!B4</f>
         <v>0.57735026918962584</v>
-      </c>
-      <c r="G3" s="5">
-        <f>'Survey-Normalised'!B$3</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="5">
-        <f>'A-Normalised'!D3</f>
-        <v>-1</v>
-      </c>
-      <c r="C4" s="5">
-        <f>'B-Normalised'!D3</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <f>'Survey-Normalised'!C$4</f>
-        <v>-0.80064076902543546</v>
-      </c>
-      <c r="E4" s="5">
-        <f>'C-Normalised'!D3</f>
-        <v>-0.14379932713576235</v>
-      </c>
-      <c r="F4" s="5">
-        <f>'D-Normalised'!D3</f>
-        <v>-1.1547005383792521</v>
-      </c>
-      <c r="G4" s="5">
-        <f>'Survey-Normalised'!B$4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5">
-        <f>'A-Normalised'!D4</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <f>'B-Normalised'!D4</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <f>'Survey-Normalised'!C$5</f>
-        <v>-0.32025630761017426</v>
-      </c>
-      <c r="E5" s="5">
-        <f>'C-Normalised'!D4</f>
-        <v>1.0641150208046437</v>
-      </c>
-      <c r="F5" s="5">
-        <f>'D-Normalised'!D4</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="G5" s="5">
-        <f>'Survey-Normalised'!B$5</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A75:A339 A3:A6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A74:A338 A2:A5">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -4073,7 +4053,7 @@
           <x14:formula1>
             <xm:f>Metadata!$A$252:$A$257</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:O2</xm:sqref>
+          <xm:sqref>B1:M1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4083,7 +4063,390 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja24"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="20">
+        <f>IF(B2&gt;0,'Indicators-Cluster-2010'!B2*B2)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
+        <f>IF(C2&gt;0,'Indicators-Cluster-2010'!C2*C2)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D3" s="20">
+        <f>IF(D2&gt;0,'Indicators-Cluster-2010'!D2*D2)</f>
+        <v>-0.28867513459481275</v>
+      </c>
+      <c r="E3" s="20">
+        <f>IF(E2&gt;0,'Indicators-Cluster-2010'!E2*E2)</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="20">
+        <f>IF(B2&gt;0,'Indicators-Cluster-2010'!B3*B2)</f>
+        <v>-1</v>
+      </c>
+      <c r="C4" s="20">
+        <f>IF(C2&gt;0,'Indicators-Cluster-2010'!C3*C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="20">
+        <f>IF(D2&gt;0,'Indicators-Cluster-2010'!D3*D2)</f>
+        <v>-0.28867513459481275</v>
+      </c>
+      <c r="E4" s="20">
+        <f>IF(E2&gt;0,'Indicators-Cluster-2010'!E3*E2)</f>
+        <v>-1.1547005383792521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="20">
+        <f>IF(B2&gt;0,'Indicators-Cluster-2010'!B4*B2)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="20">
+        <f>IF(C2&gt;0,'Indicators-Cluster-2010'!C4*C2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="20">
+        <f>IF(D2&gt;0,'Indicators-Cluster-2010'!D4*D2)</f>
+        <v>0.57735026918962506</v>
+      </c>
+      <c r="E5" s="20">
+        <f>IF(E2&gt;0,'Indicators-Cluster-2010'!E4*E2)</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A73:A337 A3:A5">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$252:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:M1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!B$3:'Indicators-Weighted-2010'!C$3)</f>
+        <v>-0.25</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0</v>
+      </c>
+      <c r="D2" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!D3)</f>
+        <v>-0.28867513459481275</v>
+      </c>
+      <c r="E2" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!E3)</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!B$4:'Indicators-Weighted-2010'!C$4)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!D4)</f>
+        <v>-0.28867513459481275</v>
+      </c>
+      <c r="E3" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!E4)</f>
+        <v>-1.1547005383792521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!B$5:'Indicators-Weighted-2010'!C$5)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!D5)</f>
+        <v>0.57735026918962506</v>
+      </c>
+      <c r="E4" s="21">
+        <f>AVERAGE('Indicators-Weighted-2010'!E5)</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$261:$A$264</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>SUM('Clusters-Grouped-2010'!B2:'Clusters-Grouped-2010'!C2)</f>
+        <v>-0.25</v>
+      </c>
+      <c r="C2" s="21">
+        <f>SUM('Clusters-Grouped-2010'!D2:'Clusters-Grouped-2010'!E2)</f>
+        <v>0.28867513459481309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="21">
+        <f>SUM('Clusters-Grouped-2010'!B3:'Clusters-Grouped-2010'!C3)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C3" s="21">
+        <f>SUM('Clusters-Grouped-2010'!D3:'Clusters-Grouped-2010'!E3)</f>
+        <v>-1.443375672974065</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="21">
+        <f>SUM('Clusters-Grouped-2010'!B4:'Clusters-Grouped-2010'!C4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="21">
+        <f>SUM('Clusters-Grouped-2010'!D4:'Clusters-Grouped-2010'!E4)</f>
+        <v>1.154700538379251</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$267:$A$268</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:C1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2">
+        <f>'Subindex-Grouped-2010'!B2*Metadata!B267+'Subindex-Grouped-2010'!C2*Metadata!B268</f>
+        <v>7.3205080756887836E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <f>'Subindex-Grouped-2010'!B3*Metadata!B267+'Subindex-Grouped-2010'!C3*Metadata!B268</f>
+        <v>-1.066025403784439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <f>'Subindex-Grouped-2010'!B4*Metadata!B267+'Subindex-Grouped-2010'!C4*Metadata!B268</f>
+        <v>0.99282032302755063</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="30"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja23"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4120,28 +4483,28 @@
         <v>204</v>
       </c>
       <c r="B2" s="5">
-        <f>'Indicators-Cluster'!B3+8</f>
-        <v>8</v>
+        <f>'A-Normalised'!D$2</f>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <f>'Indicators-Cluster'!C3+8</f>
-        <v>7</v>
+        <f>'B-Normalised'!D$2</f>
+        <v>-1</v>
       </c>
       <c r="D2" s="5">
-        <f>'Indicators-Cluster'!D3+8</f>
-        <v>9.1208970766356092</v>
+        <f>'Survey-Normalised'!C$3</f>
+        <v>1.1208970766356094</v>
       </c>
       <c r="E2" s="5">
-        <f>'Indicators-Cluster'!E3+8</f>
-        <v>7.079684306331119</v>
+        <f>'C-Normalised'!D$2</f>
+        <v>-0.92031569366888055</v>
       </c>
       <c r="F2" s="5">
-        <f>'Indicators-Cluster'!F3+8</f>
-        <v>8.5773502691896262</v>
+        <f>'D-Normalised'!D$2</f>
+        <v>0.57735026918962584</v>
       </c>
       <c r="G2" s="5">
-        <f>'Indicators-Cluster'!G3+8</f>
-        <v>7</v>
+        <f>'Survey-Normalised'!B$3</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4149,28 +4512,28 @@
         <v>78</v>
       </c>
       <c r="B3" s="5">
-        <f>'Indicators-Cluster'!B4+8</f>
-        <v>7</v>
+        <f>'A-Normalised'!D3</f>
+        <v>-1</v>
       </c>
       <c r="C3" s="5">
-        <f>'Indicators-Cluster'!C4+8</f>
-        <v>8</v>
+        <f>'B-Normalised'!D3</f>
+        <v>0</v>
       </c>
       <c r="D3" s="5">
-        <f>'Indicators-Cluster'!D4+8</f>
-        <v>7.1993592309745642</v>
+        <f>'Survey-Normalised'!C$4</f>
+        <v>-0.80064076902543546</v>
       </c>
       <c r="E3" s="5">
-        <f>'Indicators-Cluster'!E4+8</f>
-        <v>7.8562006728642375</v>
+        <f>'C-Normalised'!D3</f>
+        <v>-0.14379932713576235</v>
       </c>
       <c r="F3" s="5">
-        <f>'Indicators-Cluster'!F4+8</f>
-        <v>6.8452994616207476</v>
+        <f>'D-Normalised'!D3</f>
+        <v>-1.1547005383792521</v>
       </c>
       <c r="G3" s="5">
-        <f>'Indicators-Cluster'!G4+8</f>
-        <v>8</v>
+        <f>'Survey-Normalised'!B$4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4178,33 +4541,33 @@
         <v>48</v>
       </c>
       <c r="B4" s="5">
-        <f>'Indicators-Cluster'!B5+8</f>
-        <v>9</v>
+        <f>'A-Normalised'!D4</f>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <f>'Indicators-Cluster'!C5+8</f>
-        <v>9</v>
+        <f>'B-Normalised'!D4</f>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <f>'Indicators-Cluster'!D5+8</f>
-        <v>7.6797436923898257</v>
+        <f>'Survey-Normalised'!C$5</f>
+        <v>-0.32025630761017426</v>
       </c>
       <c r="E4" s="5">
-        <f>'Indicators-Cluster'!E5+8</f>
-        <v>9.0641150208046444</v>
+        <f>'C-Normalised'!D4</f>
+        <v>1.0641150208046437</v>
       </c>
       <c r="F4" s="5">
-        <f>'Indicators-Cluster'!F5+8</f>
-        <v>8.5773502691896262</v>
+        <f>'D-Normalised'!D4</f>
+        <v>0.57735026918962584</v>
       </c>
       <c r="G4" s="5">
-        <f>'Indicators-Cluster'!G5+8</f>
-        <v>9</v>
+        <f>'Survey-Normalised'!B$5</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A73:A337 A2:A4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A74:A338 A2:A5">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -4225,13 +4588,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja25"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4287,28 +4650,28 @@
         <v>204</v>
       </c>
       <c r="B3" s="20">
-        <f>IF(B2&gt;0,'Indicators-Adjusted'!B2*B2)</f>
-        <v>8</v>
+        <f>IF(B2&gt;0,'Indicators-Cluster-2012'!B2*B2)</f>
+        <v>0</v>
       </c>
       <c r="C3" s="20">
-        <f>IF(C2&gt;0,'Indicators-Adjusted'!C2*C2)</f>
-        <v>3.5</v>
+        <f>IF(C2&gt;0,'Indicators-Cluster-2012'!C2*C2)</f>
+        <v>-0.5</v>
       </c>
       <c r="D3" s="20">
-        <f>IF(D2&gt;0,'Indicators-Adjusted'!D2*D2)</f>
-        <v>9.1208970766356092</v>
+        <f>IF(D2&gt;0,'Indicators-Cluster-2012'!D2*D2)</f>
+        <v>1.1208970766356094</v>
       </c>
       <c r="E3" s="20">
-        <f>IF(E2&gt;0,'Indicators-Adjusted'!E2*E2)</f>
-        <v>3.5398421531655595</v>
+        <f>IF(E2&gt;0,'Indicators-Cluster-2012'!E2*E2)</f>
+        <v>-0.46015784683444028</v>
       </c>
       <c r="F3" s="20">
-        <f>IF(F2&gt;0,'Indicators-Adjusted'!F2*F2)</f>
-        <v>8.5773502691896262</v>
+        <f>IF(F2&gt;0,'Indicators-Cluster-2012'!F2*F2)</f>
+        <v>0.57735026918962584</v>
       </c>
       <c r="G3" s="20">
-        <f>IF(G2&gt;0,'Indicators-Adjusted'!G2*G2)</f>
-        <v>3.5</v>
+        <f>IF(G2&gt;0,'Indicators-Cluster-2012'!G2*G2)</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4316,28 +4679,28 @@
         <v>78</v>
       </c>
       <c r="B4" s="20">
-        <f>IF(B2&gt;0,'Indicators-Adjusted'!B3*B2)</f>
-        <v>7</v>
+        <f>IF(B2&gt;0,'Indicators-Cluster-2012'!B3*B2)</f>
+        <v>-1</v>
       </c>
       <c r="C4" s="20">
-        <f>IF(C2&gt;0,'Indicators-Adjusted'!C3*C2)</f>
-        <v>4</v>
+        <f>IF(C2&gt;0,'Indicators-Cluster-2012'!C3*C2)</f>
+        <v>0</v>
       </c>
       <c r="D4" s="20">
-        <f>IF(D2&gt;0,'Indicators-Adjusted'!D3*D2)</f>
-        <v>7.1993592309745642</v>
+        <f>IF(D2&gt;0,'Indicators-Cluster-2012'!D3*D2)</f>
+        <v>-0.80064076902543546</v>
       </c>
       <c r="E4" s="20">
-        <f>IF(E2&gt;0,'Indicators-Adjusted'!E3*E2)</f>
-        <v>3.9281003364321188</v>
+        <f>IF(E2&gt;0,'Indicators-Cluster-2012'!E3*E2)</f>
+        <v>-7.1899663567881175E-2</v>
       </c>
       <c r="F4" s="20">
-        <f>IF(F2&gt;0,'Indicators-Adjusted'!F3*F2)</f>
-        <v>6.8452994616207476</v>
+        <f>IF(F2&gt;0,'Indicators-Cluster-2012'!F3*F2)</f>
+        <v>-1.1547005383792521</v>
       </c>
       <c r="G4" s="20">
-        <f>IF(G2&gt;0,'Indicators-Adjusted'!G3*G2)</f>
-        <v>4</v>
+        <f>IF(G2&gt;0,'Indicators-Cluster-2012'!G3*G2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4345,28 +4708,28 @@
         <v>48</v>
       </c>
       <c r="B5" s="20">
-        <f>IF(B2&gt;0,'Indicators-Adjusted'!B4*B2)</f>
-        <v>9</v>
+        <f>IF(B2&gt;0,'Indicators-Cluster-2012'!B4*B2)</f>
+        <v>1</v>
       </c>
       <c r="C5" s="20">
-        <f>IF(C2&gt;0,'Indicators-Adjusted'!C4*C2)</f>
-        <v>4.5</v>
+        <f>IF(C2&gt;0,'Indicators-Cluster-2012'!C4*C2)</f>
+        <v>0.5</v>
       </c>
       <c r="D5" s="20">
-        <f>IF(D2&gt;0,'Indicators-Adjusted'!D4*D2)</f>
-        <v>7.6797436923898257</v>
+        <f>IF(D2&gt;0,'Indicators-Cluster-2012'!D4*D2)</f>
+        <v>-0.32025630761017426</v>
       </c>
       <c r="E5" s="20">
-        <f>IF(E2&gt;0,'Indicators-Adjusted'!E4*E2)</f>
-        <v>4.5320575104023222</v>
+        <f>IF(E2&gt;0,'Indicators-Cluster-2012'!E4*E2)</f>
+        <v>0.53205751040232185</v>
       </c>
       <c r="F5" s="20">
-        <f>IF(F2&gt;0,'Indicators-Adjusted'!F4*F2)</f>
-        <v>8.5773502691896262</v>
+        <f>IF(F2&gt;0,'Indicators-Cluster-2012'!F4*F2)</f>
+        <v>0.57735026918962584</v>
       </c>
       <c r="G5" s="20">
-        <f>IF(G2&gt;0,'Indicators-Adjusted'!G4*G2)</f>
-        <v>4.5</v>
+        <f>IF(G2&gt;0,'Indicators-Cluster-2012'!G4*G2)</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4392,7 +4755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:E4"/>
@@ -4425,20 +4788,20 @@
         <v>204</v>
       </c>
       <c r="B2" s="21">
-        <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
-        <v>5.75</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!B$3:'Indicators-Weighted-2012'!C$3)</f>
+        <v>-0.25</v>
       </c>
       <c r="C2" s="21">
-        <f>AVERAGE('Indicators-Weighted'!D3)</f>
-        <v>9.1208970766356092</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!D3)</f>
+        <v>1.1208970766356094</v>
       </c>
       <c r="D2" s="21">
-        <f>AVERAGE('Indicators-Weighted'!E3)</f>
-        <v>3.5398421531655595</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!E3)</f>
+        <v>-0.46015784683444028</v>
       </c>
       <c r="E2" s="21">
-        <f>AVERAGE('Indicators-Weighted'!G3:'Indicators-Weighted'!F3)</f>
-        <v>6.0386751345948131</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!G3:'Indicators-Weighted-2012'!F3)</f>
+        <v>3.8675134594812921E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4446,20 +4809,20 @@
         <v>78</v>
       </c>
       <c r="B3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
-        <v>5.5</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!B$4:'Indicators-Weighted-2012'!C$4)</f>
+        <v>-0.5</v>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!D4)</f>
-        <v>7.1993592309745642</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!D4)</f>
+        <v>-0.80064076902543546</v>
       </c>
       <c r="D3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!E4)</f>
-        <v>3.9281003364321188</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!E4)</f>
+        <v>-7.1899663567881175E-2</v>
       </c>
       <c r="E3" s="21">
-        <f>AVERAGE('Indicators-Weighted'!G4:'Indicators-Weighted'!F4)</f>
-        <v>5.4226497308103738</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!G4:'Indicators-Weighted-2012'!F4)</f>
+        <v>-0.57735026918962606</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4467,20 +4830,20 @@
         <v>48</v>
       </c>
       <c r="B4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!B$5:'Indicators-Weighted'!C$5)</f>
-        <v>6.75</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!B$5:'Indicators-Weighted-2012'!C$5)</f>
+        <v>0.75</v>
       </c>
       <c r="C4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!D5)</f>
-        <v>7.6797436923898257</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!D5)</f>
+        <v>-0.32025630761017426</v>
       </c>
       <c r="D4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!E5)</f>
-        <v>4.5320575104023222</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!E5)</f>
+        <v>0.53205751040232185</v>
       </c>
       <c r="E4" s="21">
-        <f>AVERAGE('Indicators-Weighted'!G5:'Indicators-Weighted'!F5)</f>
-        <v>6.5386751345948131</v>
+        <f>AVERAGE('Indicators-Weighted-2012'!G5:'Indicators-Weighted-2012'!F5)</f>
+        <v>0.53867513459481287</v>
       </c>
     </row>
   </sheetData>
@@ -4506,7 +4869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja27"/>
   <dimension ref="A1:C4"/>
@@ -4533,12 +4896,12 @@
         <v>204</v>
       </c>
       <c r="B2" s="21">
-        <f>AVERAGE('Clusters-Grouped'!B2:'Clusters-Grouped'!C2)</f>
-        <v>7.4354485383178046</v>
+        <f>SUM('Clusters-Grouped-2012'!B2:'Clusters-Grouped-2012'!C2)</f>
+        <v>0.87089707663560945</v>
       </c>
       <c r="C2" s="21">
-        <f>AVERAGE('Clusters-Grouped'!D2:'Clusters-Grouped'!E2)</f>
-        <v>4.7892586438801867</v>
+        <f>SUM('Clusters-Grouped-2012'!D2:'Clusters-Grouped-2012'!E2)</f>
+        <v>-0.42148271223962736</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4546,12 +4909,12 @@
         <v>78</v>
       </c>
       <c r="B3" s="21">
-        <f>AVERAGE('Clusters-Grouped'!B3:'Clusters-Grouped'!C3)</f>
-        <v>6.3496796154872825</v>
+        <f>SUM('Clusters-Grouped-2012'!B3:'Clusters-Grouped-2012'!C3)</f>
+        <v>-1.3006407690254354</v>
       </c>
       <c r="C3" s="21">
-        <f>AVERAGE('Clusters-Grouped'!D3:'Clusters-Grouped'!E3)</f>
-        <v>4.6753750336212461</v>
+        <f>SUM('Clusters-Grouped-2012'!D3:'Clusters-Grouped-2012'!E3)</f>
+        <v>-0.6492499327575072</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4559,12 +4922,12 @@
         <v>48</v>
       </c>
       <c r="B4" s="21">
-        <f>AVERAGE('Clusters-Grouped'!B4:'Clusters-Grouped'!C4)</f>
-        <v>7.2148718461949128</v>
+        <f>SUM('Clusters-Grouped-2012'!B4:'Clusters-Grouped-2012'!C4)</f>
+        <v>0.42974369238982574</v>
       </c>
       <c r="C4" s="21">
-        <f>AVERAGE('Clusters-Grouped'!D4:'Clusters-Grouped'!E4)</f>
-        <v>5.5353663224985681</v>
+        <f>SUM('Clusters-Grouped-2012'!D4:'Clusters-Grouped-2012'!E4)</f>
+        <v>1.0707326449971348</v>
       </c>
     </row>
   </sheetData>
@@ -4590,7 +4953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja28"/>
   <dimension ref="A1:B4"/>
@@ -4614,8 +4977,8 @@
         <v>204</v>
       </c>
       <c r="B2">
-        <f>'Subindex-Grouped'!B2*Metadata!B267+'Subindex-Grouped'!C2*Metadata!B268</f>
-        <v>5.8477346016552341</v>
+        <f>'Subindex-Grouped-2012'!B2*Metadata!B267+'Subindex-Grouped-2012'!C2*Metadata!B268</f>
+        <v>9.5469203310467377E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4623,8 +4986,8 @@
         <v>78</v>
       </c>
       <c r="B3">
-        <f>'Subindex-Grouped'!B3*Metadata!B267+'Subindex-Grouped'!C3*Metadata!B268</f>
-        <v>5.3450968663676601</v>
+        <f>'Subindex-Grouped-2012'!B3*Metadata!B267+'Subindex-Grouped-2012'!C3*Metadata!B268</f>
+        <v>-0.9098062672646785</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4632,331 +4995,14 @@
         <v>48</v>
       </c>
       <c r="B4">
-        <f>'Subindex-Grouped'!B4*Metadata!B267+'Subindex-Grouped'!C4*Metadata!B268</f>
-        <v>6.2071685319771062</v>
+        <f>'Subindex-Grouped-2012'!B4*Metadata!B267+'Subindex-Grouped-2012'!C4*Metadata!B268</f>
+        <v>0.81433706395421113</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
-      <formula1>countries</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja29"/>
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G1" t="s">
-        <v>265</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F2" t="s">
-        <v>264</v>
-      </c>
-      <c r="G2" t="s">
-        <v>270</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="22">
-        <f>RANK('Clusters-Grouped'!B2,'Clusters-Grouped'!B$2:B$4)</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="22">
-        <f>RANK('Clusters-Grouped'!C2,'Clusters-Grouped'!C$2:C$4)</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="22">
-        <f>RANK('Subindex-Grouped'!B2,'Subindex-Grouped'!B$2:B$4)</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="22">
-        <f>RANK('Clusters-Grouped'!D2,'Clusters-Grouped'!D$2:D$4)</f>
-        <v>3</v>
-      </c>
-      <c r="F3" s="22">
-        <f>RANK('Clusters-Grouped'!E2,'Clusters-Grouped'!E$2:E$4)</f>
-        <v>2</v>
-      </c>
-      <c r="G3" s="22">
-        <f>RANK('Subindex-Grouped'!C2,'Subindex-Grouped'!C$2:C$4)</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="24">
-        <f>RANK(Composite!B2,Composite!B$2:B$4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="22">
-        <f>RANK('Clusters-Grouped'!B3,'Clusters-Grouped'!B$2:B$4)</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="22">
-        <f>RANK('Clusters-Grouped'!C3,'Clusters-Grouped'!C$2:C$4)</f>
-        <v>3</v>
-      </c>
-      <c r="D4" s="22">
-        <f>RANK('Subindex-Grouped'!B3,'Subindex-Grouped'!B$2:B$4)</f>
-        <v>3</v>
-      </c>
-      <c r="E4" s="22">
-        <f>RANK('Clusters-Grouped'!D3,'Clusters-Grouped'!D$2:D$4)</f>
-        <v>2</v>
-      </c>
-      <c r="F4" s="22">
-        <f>RANK('Clusters-Grouped'!E3,'Clusters-Grouped'!E$2:E$4)</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="22">
-        <f>RANK('Subindex-Grouped'!C3,'Subindex-Grouped'!C$2:C$4)</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="24">
-        <f>RANK(Composite!B3,Composite!B$2:B$4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="22">
-        <f>RANK('Clusters-Grouped'!B4,'Clusters-Grouped'!B$2:B$4)</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="22">
-        <f>RANK('Clusters-Grouped'!C4,'Clusters-Grouped'!C$2:C$4)</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="22">
-        <f>RANK('Subindex-Grouped'!B4,'Subindex-Grouped'!B$2:B$4)</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="22">
-        <f>RANK('Clusters-Grouped'!D4,'Clusters-Grouped'!D$2:D$4)</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="22">
-        <f>RANK('Clusters-Grouped'!E4,'Clusters-Grouped'!E$2:E$4)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="22">
-        <f>RANK('Subindex-Grouped'!C4,'Subindex-Grouped'!C$2:C$4)</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="24">
-        <f>RANK(Composite!B4,Composite!B$2:B$4)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja30"/>
-  <dimension ref="A2:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="5">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="5">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="13">
-        <v>8</v>
-      </c>
-      <c r="C5" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>AVERAGE(B3:B5)</f>
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <f>AVERAGE(C3:C5)</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="D7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <f>STDEV(B3:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <f>STDEV(C3:C5)</f>
-        <v>2.0816659994661335</v>
-      </c>
-      <c r="D8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
-      <formula1>countries</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="5">
-        <f>('Survey-Raw'!B$3-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
-        <v>-1</v>
-      </c>
-      <c r="C3" s="5">
-        <f>('Survey-Raw'!C$3-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
-        <v>1.1208970766356094</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="5">
-        <f>('Survey-Raw'!B$4-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <f>('Survey-Raw'!C$4-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
-        <v>-0.80064076902543546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5">
-        <f>('Survey-Raw'!B$5-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <f>('Survey-Raw'!C$5-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
-        <v>-0.32025630761017426</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
       <formula1>countries</formula1>
     </dataValidation>
   </dataValidations>
@@ -5051,6 +5097,323 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja29"/>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="22">
+        <f>RANK('Clusters-Grouped-2012'!B2,'Clusters-Grouped-2012'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="22">
+        <f>RANK('Clusters-Grouped-2012'!C2,'Clusters-Grouped-2012'!C$2:C$4)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="22">
+        <f>RANK('Subindex-Grouped-2012'!B2,'Subindex-Grouped-2012'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <f>RANK('Clusters-Grouped-2012'!D2,'Clusters-Grouped-2012'!D$2:D$4)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="22">
+        <f>RANK('Clusters-Grouped-2012'!E2,'Clusters-Grouped-2012'!E$2:E$4)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="22">
+        <f>RANK('Subindex-Grouped-2012'!C2,'Subindex-Grouped-2012'!C$2:C$4)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="24">
+        <f>RANK('Composite-2012'!B2,'Composite-2012'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="22">
+        <f>RANK('Clusters-Grouped-2012'!B3,'Clusters-Grouped-2012'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="22">
+        <f>RANK('Clusters-Grouped-2012'!C3,'Clusters-Grouped-2012'!C$2:C$4)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="22">
+        <f>RANK('Subindex-Grouped-2012'!B3,'Subindex-Grouped-2012'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="22">
+        <f>RANK('Clusters-Grouped-2012'!D3,'Clusters-Grouped-2012'!D$2:D$4)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="22">
+        <f>RANK('Clusters-Grouped-2012'!E3,'Clusters-Grouped-2012'!E$2:E$4)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="22">
+        <f>RANK('Subindex-Grouped-2012'!C3,'Subindex-Grouped-2012'!C$2:C$4)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="24">
+        <f>RANK('Composite-2012'!B3,'Composite-2012'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="22">
+        <f>RANK('Clusters-Grouped-2012'!B4,'Clusters-Grouped-2012'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <f>RANK('Clusters-Grouped-2012'!C4,'Clusters-Grouped-2012'!C$2:C$4)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="22">
+        <f>RANK('Subindex-Grouped-2012'!B4,'Subindex-Grouped-2012'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="22">
+        <f>RANK('Clusters-Grouped-2012'!D4,'Clusters-Grouped-2012'!D$2:D$4)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <f>RANK('Clusters-Grouped-2012'!E4,'Clusters-Grouped-2012'!E$2:E$4)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="22">
+        <f>RANK('Subindex-Grouped-2012'!C4,'Subindex-Grouped-2012'!C$2:C$4)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="24">
+        <f>RANK('Composite-2012'!B4,'Composite-2012'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja30"/>
+  <dimension ref="A2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="5">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="13">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f>AVERAGE(B3:B5)</f>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C3:C5)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>STDEV(B3:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>STDEV(C3:C5)</f>
+        <v>2.0816659994661335</v>
+      </c>
+      <c r="D8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="5">
+        <f>('Survey-Raw'!B$3-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
+        <v>-1</v>
+      </c>
+      <c r="C3" s="5">
+        <f>('Survey-Raw'!C$3-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
+        <v>1.1208970766356094</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="5">
+        <f>('Survey-Raw'!B$4-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <f>('Survey-Raw'!C$4-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
+        <v>-0.80064076902543546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5">
+        <f>('Survey-Raw'!B$5-'Survey-Raw'!B$7)/'Survey-Raw'!B$8</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <f>('Survey-Raw'!C$5-'Survey-Raw'!C$7)/'Survey-Raw'!C$8</f>
+        <v>-0.32025630761017426</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A5">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>